<commit_message>
update des fichiers Ajout des nom/prénom, ajout tableau de gantt, ajout tableau de synthèse version FR
</commit_message>
<xml_diff>
--- a/VILLEMY-EMELINE-Tableau-de-synthèse-Epreuve-E4-BTS-SIO-2024.xlsx
+++ b/VILLEMY-EMELINE-Tableau-de-synthèse-Epreuve-E4-BTS-SIO-2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flamb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flamb\Desktop\git clone\Portfolio-Villemy-Emeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B07BC7F-44B1-4CEC-9B78-C14415FDB1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5689EB62-64DB-487E-9AF3-F936F85C1863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -245,15 +245,6 @@
     <t>Création de compte QAD, modification et gestion de droits</t>
   </si>
   <si>
-    <t>Onboarding and Offboarding of employees</t>
-  </si>
-  <si>
-    <t>Helpdesk</t>
-  </si>
-  <si>
-    <t>Hardware management</t>
-  </si>
-  <si>
     <t>Gestion de la flotte mobile</t>
   </si>
   <si>
@@ -261,6 +252,15 @@
   </si>
   <si>
     <t>SESSION 2024</t>
+  </si>
+  <si>
+    <t>Support informatique (Helpdesk)</t>
+  </si>
+  <si>
+    <t>Arrivées et Départs des salariés</t>
+  </si>
+  <si>
+    <t>Gestion du matériel informatique</t>
   </si>
 </sst>
 </file>
@@ -802,14 +802,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -842,30 +866,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4098,7 +4098,7 @@
   <dimension ref="A1:AQ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
@@ -4111,56 +4111,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="12" t="s">
         <v>2</v>
       </c>
@@ -4172,22 +4172,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -4210,8 +4210,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="20" t="s">
         <v>13</v>
       </c>
@@ -4267,16 +4267,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -4804,16 +4804,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -5182,16 +5182,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -5233,7 +5233,7 @@
         <v>51</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -5279,10 +5279,10 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -5328,10 +5328,10 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -5377,10 +5377,10 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -5426,10 +5426,10 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -5656,11 +5656,6 @@
     <row r="81" customFormat="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -5668,6 +5663,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -5679,71 +5679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="923d05d6-6373-43a5-b79f-b15157901251" xsi:nil="true"/>
-    <Templates xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <TeamsChannelId xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Invited_Students xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Distribution_Groups xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <CultureName xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <LMS_Mappings xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Invited_Teachers xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <NotebookType xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <FolderType xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Teachers xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <AppVersion xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Math_Settings xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-    <Owner xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <IsNotebookLocked xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD1390579AA2DB42B60BD32A8BA9EE87" ma:contentTypeVersion="31" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="ba849a583d5760fc5e6291fbe9c29db4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xmlns:ns3="923d05d6-6373-43a5-b79f-b15157901251" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31a5bc707d5d173ae01fcf70c38e89af" ns2:_="" ns3:_="">
     <xsd:import namespace="5f4da1f7-5808-483f-b15f-b2962f27b5ab"/>
@@ -6126,10 +6061,86 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="923d05d6-6373-43a5-b79f-b15157901251" xsi:nil="true"/>
+    <Templates xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <TeamsChannelId xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Invited_Students xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Distribution_Groups xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <CultureName xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <LMS_Mappings xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Invited_Teachers xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <NotebookType xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <FolderType xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Teachers xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <AppVersion xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Math_Settings xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+    <Owner xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <IsNotebookLocked xmlns="5f4da1f7-5808-483f-b15f-b2962f27b5ab" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E082B0F-951B-4981-B94B-5E1A792B3DE7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F3853F1-961F-427F-9C65-EBA82BA2BAC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5f4da1f7-5808-483f-b15f-b2962f27b5ab"/>
+    <ds:schemaRef ds:uri="923d05d6-6373-43a5-b79f-b15157901251"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6146,20 +6157,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F3853F1-961F-427F-9C65-EBA82BA2BAC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E082B0F-951B-4981-B94B-5E1A792B3DE7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5f4da1f7-5808-483f-b15f-b2962f27b5ab"/>
-    <ds:schemaRef ds:uri="923d05d6-6373-43a5-b79f-b15157901251"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>